<commit_message>
doc: updated data dictionary
</commit_message>
<xml_diff>
--- a/next_mui/data_dictionary.xlsx
+++ b/next_mui/data_dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fixtures_&lt;season_id&gt;" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t xml:space="preserve">team_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strign</t>
   </si>
 </sst>
 </file>
@@ -230,8 +227,8 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -361,10 +358,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -372,10 +369,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -400,13 +397,13 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,13 +429,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>